<commit_message>
1000exp new_cu with lambda
</commit_message>
<xml_diff>
--- a/results/new_cu_diffgoal_path/15x15/new_cu_diffgoal_path_15x15_True_2_1000.xlsx
+++ b/results/new_cu_diffgoal_path/15x15/new_cu_diffgoal_path_15x15_True_2_1000.xlsx
@@ -518,40 +518,40 @@
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>54.069</v>
+        <v>54.114</v>
       </c>
       <c r="D2" t="n">
-        <v>54.069</v>
+        <v>54.114</v>
       </c>
       <c r="E2" t="n">
-        <v>3.17825061</v>
+        <v>3.16948242</v>
       </c>
       <c r="F2" t="n">
-        <v>0.00133787</v>
+        <v>0.00135841</v>
       </c>
       <c r="G2" t="n">
-        <v>0.07169933000000001</v>
+        <v>0.07295569</v>
       </c>
       <c r="H2" t="n">
-        <v>3.90818598</v>
+        <v>3.97650341</v>
       </c>
       <c r="I2" t="n">
-        <v>7.01023411751579</v>
+        <v>6.551482727285933</v>
       </c>
       <c r="J2" t="n">
-        <v>7.01023411751579</v>
+        <v>6.551482727285933</v>
       </c>
       <c r="K2" t="n">
-        <v>0.4138050426220387</v>
+        <v>0.3907925152580654</v>
       </c>
       <c r="L2" t="n">
-        <v>0.0001462147114412289</v>
+        <v>0.0001665157632159772</v>
       </c>
       <c r="M2" t="n">
-        <v>0.007553342586917089</v>
+        <v>0.008893789057972293</v>
       </c>
       <c r="N2" t="n">
-        <v>0.8345269440073902</v>
+        <v>0.8448462905931474</v>
       </c>
       <c r="O2" t="n">
         <v>0.15</v>
@@ -565,40 +565,40 @@
         <v>1</v>
       </c>
       <c r="C3" t="n">
-        <v>90.059</v>
+        <v>90.295</v>
       </c>
       <c r="D3" t="n">
-        <v>90.059</v>
+        <v>90.295</v>
       </c>
       <c r="E3" t="n">
-        <v>1.91107263</v>
+        <v>1.904231</v>
       </c>
       <c r="F3" t="n">
-        <v>0.0009027800000000001</v>
+        <v>0.000943</v>
       </c>
       <c r="G3" t="n">
-        <v>0.08052294</v>
+        <v>0.08433705000000001</v>
       </c>
       <c r="H3" t="n">
-        <v>7.314089279999999</v>
+        <v>7.67577954</v>
       </c>
       <c r="I3" t="n">
-        <v>12.08642215879458</v>
+        <v>11.89283037861107</v>
       </c>
       <c r="J3" t="n">
-        <v>12.08642215879458</v>
+        <v>11.89283037861107</v>
       </c>
       <c r="K3" t="n">
-        <v>0.2625993418524205</v>
+        <v>0.2527369708595069</v>
       </c>
       <c r="L3" t="n">
-        <v>0.0001330374780675377</v>
+        <v>0.0001822350394671936</v>
       </c>
       <c r="M3" t="n">
-        <v>0.01143470110434662</v>
+        <v>0.01559989991233196</v>
       </c>
       <c r="N3" t="n">
-        <v>1.735984363536182</v>
+        <v>2.005840126932154</v>
       </c>
       <c r="O3" t="n">
         <v>0.85</v>
@@ -612,40 +612,40 @@
         <v>1</v>
       </c>
       <c r="C4" t="n">
-        <v>27.046</v>
+        <v>27.812</v>
       </c>
       <c r="D4" t="n">
-        <v>54.078</v>
+        <v>55.605</v>
       </c>
       <c r="E4" t="n">
-        <v>3.25338949</v>
+        <v>3.104128</v>
       </c>
       <c r="F4" t="n">
-        <v>0.00252739</v>
+        <v>0.00264691</v>
       </c>
       <c r="G4" t="n">
-        <v>0.03362475000000001</v>
+        <v>0.0365285</v>
       </c>
       <c r="H4" t="n">
-        <v>0.93228702</v>
+        <v>1.03036605</v>
       </c>
       <c r="I4" t="n">
-        <v>5.543339481992115</v>
+        <v>4.142924066383527</v>
       </c>
       <c r="J4" t="n">
-        <v>11.08777952769872</v>
+        <v>8.279222217124053</v>
       </c>
       <c r="K4" t="n">
-        <v>0.6504573511170907</v>
+        <v>0.4427500415151439</v>
       </c>
       <c r="L4" t="n">
-        <v>0.0003879244427375946</v>
+        <v>0.0005123196495580892</v>
       </c>
       <c r="M4" t="n">
-        <v>0.005954293253245564</v>
+        <v>0.007658787474240003</v>
       </c>
       <c r="N4" t="n">
-        <v>0.341152542880503</v>
+        <v>0.3245784489303126</v>
       </c>
       <c r="O4" t="n">
         <v>0.15</v>
@@ -659,40 +659,40 @@
         <v>1</v>
       </c>
       <c r="C5" t="n">
-        <v>48.528</v>
+        <v>46.208</v>
       </c>
       <c r="D5" t="n">
-        <v>94.90900000000001</v>
+        <v>90.684</v>
       </c>
       <c r="E5" t="n">
-        <v>1.83129985</v>
+        <v>1.91382706</v>
       </c>
       <c r="F5" t="n">
-        <v>0.00154295</v>
+        <v>0.00166198</v>
       </c>
       <c r="G5" t="n">
-        <v>0.03694269</v>
+        <v>0.03787804</v>
       </c>
       <c r="H5" t="n">
-        <v>1.82836536</v>
+        <v>1.78094815</v>
       </c>
       <c r="I5" t="n">
-        <v>8.870394574081802</v>
+        <v>8.199632306998282</v>
       </c>
       <c r="J5" t="n">
-        <v>16.14848266842716</v>
+        <v>15.03117028311768</v>
       </c>
       <c r="K5" t="n">
-        <v>0.3064602012516939</v>
+        <v>0.3118262287250341</v>
       </c>
       <c r="L5" t="n">
-        <v>0.0001991221914984544</v>
+        <v>0.0002498441548279681</v>
       </c>
       <c r="M5" t="n">
-        <v>0.005546277946782235</v>
+        <v>0.006012809795764376</v>
       </c>
       <c r="N5" t="n">
-        <v>0.5994602327416799</v>
+        <v>0.5670590400082981</v>
       </c>
       <c r="O5" t="n">
         <v>0.85</v>
@@ -706,40 +706,40 @@
         <v>1</v>
       </c>
       <c r="C6" t="n">
-        <v>14.412</v>
+        <v>13.787</v>
       </c>
       <c r="D6" t="n">
-        <v>57.596</v>
+        <v>55.081</v>
       </c>
       <c r="E6" t="n">
-        <v>3.12679938</v>
+        <v>3.21703234</v>
       </c>
       <c r="F6" t="n">
-        <v>0.00429857</v>
+        <v>0.00435844</v>
       </c>
       <c r="G6" t="n">
-        <v>0.01526991</v>
+        <v>0.01488329</v>
       </c>
       <c r="H6" t="n">
-        <v>0.23138585</v>
+        <v>0.21439266</v>
       </c>
       <c r="I6" t="n">
-        <v>3.686983841821096</v>
+        <v>3.259794051356198</v>
       </c>
       <c r="J6" t="n">
-        <v>14.72894177209367</v>
+        <v>13.04640362887979</v>
       </c>
       <c r="K6" t="n">
-        <v>0.7895720725144161</v>
+        <v>0.656420880163054</v>
       </c>
       <c r="L6" t="n">
-        <v>0.0005525712534054681</v>
+        <v>0.0006457398441681808</v>
       </c>
       <c r="M6" t="n">
-        <v>0.003552977165510445</v>
+        <v>0.003572530258563019</v>
       </c>
       <c r="N6" t="n">
-        <v>0.1130356410103296</v>
+        <v>0.1058296747381356</v>
       </c>
       <c r="O6" t="n">
         <v>0.15</v>
@@ -753,40 +753,40 @@
         <v>1</v>
       </c>
       <c r="C7" t="n">
-        <v>25.316</v>
+        <v>24.351</v>
       </c>
       <c r="D7" t="n">
-        <v>93.711</v>
+        <v>90.449</v>
       </c>
       <c r="E7" t="n">
-        <v>1.85902356</v>
+        <v>1.92385209</v>
       </c>
       <c r="F7" t="n">
-        <v>0.00289656</v>
+        <v>0.00313757</v>
       </c>
       <c r="G7" t="n">
-        <v>0.01808876</v>
+        <v>0.01886938</v>
       </c>
       <c r="H7" t="n">
-        <v>0.47248698</v>
+        <v>0.4741455</v>
       </c>
       <c r="I7" t="n">
-        <v>5.427116877090229</v>
+        <v>5.201043150162268</v>
       </c>
       <c r="J7" t="n">
-        <v>16.34682530945069</v>
+        <v>15.66961824474151</v>
       </c>
       <c r="K7" t="n">
-        <v>0.3285856557732036</v>
+        <v>0.3288887290705498</v>
       </c>
       <c r="L7" t="n">
-        <v>0.0004357433173769148</v>
+        <v>0.000655178642931952</v>
       </c>
       <c r="M7" t="n">
-        <v>0.003690057640171463</v>
+        <v>0.004816035507926994</v>
       </c>
       <c r="N7" t="n">
-        <v>0.1946734041119848</v>
+        <v>0.2096587577418312</v>
       </c>
       <c r="O7" t="n">
         <v>0.85</v>
@@ -800,40 +800,40 @@
         <v>1</v>
       </c>
       <c r="C8" t="n">
-        <v>9.064</v>
+        <v>9.026</v>
       </c>
       <c r="D8" t="n">
-        <v>54.302</v>
+        <v>54.047</v>
       </c>
       <c r="E8" t="n">
-        <v>3.30350598</v>
+        <v>3.2465932</v>
       </c>
       <c r="F8" t="n">
-        <v>0.006348029999999999</v>
+        <v>0.00649477</v>
       </c>
       <c r="G8" t="n">
-        <v>0.00951017</v>
+        <v>0.00973795</v>
       </c>
       <c r="H8" t="n">
-        <v>0.09107359</v>
+        <v>0.09139376</v>
       </c>
       <c r="I8" t="n">
-        <v>2.335671072595488</v>
+        <v>1.854929854405488</v>
       </c>
       <c r="J8" t="n">
-        <v>14.01039211039745</v>
+        <v>11.1118073805868</v>
       </c>
       <c r="K8" t="n">
-        <v>0.7884226132480729</v>
+        <v>0.6145973977206909</v>
       </c>
       <c r="L8" t="n">
-        <v>0.001053982304309611</v>
+        <v>0.00153800201472472</v>
       </c>
       <c r="M8" t="n">
-        <v>0.002621400849453115</v>
+        <v>0.002884756439843269</v>
       </c>
       <c r="N8" t="n">
-        <v>0.04945781042690956</v>
+        <v>0.04736172435623935</v>
       </c>
       <c r="O8" t="n">
         <v>0.15</v>
@@ -844,43 +844,43 @@
         <v>6</v>
       </c>
       <c r="B9" t="n">
-        <v>1</v>
+        <v>0.99995556</v>
       </c>
       <c r="C9" t="n">
-        <v>17.186</v>
+        <v>16.821</v>
       </c>
       <c r="D9" t="n">
-        <v>87.908</v>
+        <v>86.29600000000001</v>
       </c>
       <c r="E9" t="n">
-        <v>1.98769757</v>
+        <v>2.01509231</v>
       </c>
       <c r="F9" t="n">
-        <v>0.00395629</v>
+        <v>0.004107620000000001</v>
       </c>
       <c r="G9" t="n">
-        <v>0.01114935</v>
+        <v>0.01131171</v>
       </c>
       <c r="H9" t="n">
-        <v>0.19931739</v>
+        <v>0.19793911</v>
       </c>
       <c r="I9" t="n">
-        <v>4.144705367403404</v>
+        <v>4.211020267309538</v>
       </c>
       <c r="J9" t="n">
-        <v>16.17173648873432</v>
+        <v>14.80106264615671</v>
       </c>
       <c r="K9" t="n">
-        <v>0.367135147468479</v>
+        <v>0.3395036868161016</v>
       </c>
       <c r="L9" t="n">
-        <v>0.0005622669116887282</v>
+        <v>0.000663986455896213</v>
       </c>
       <c r="M9" t="n">
-        <v>0.002346620613948025</v>
+        <v>0.00246834225531821</v>
       </c>
       <c r="N9" t="n">
-        <v>0.08966289475018573</v>
+        <v>0.09679939926366127</v>
       </c>
       <c r="O9" t="n">
         <v>0.85</v>
@@ -894,40 +894,40 @@
         <v>1</v>
       </c>
       <c r="C10" t="n">
-        <v>6.952</v>
+        <v>6.91</v>
       </c>
       <c r="D10" t="n">
-        <v>55.473</v>
+        <v>55.089</v>
       </c>
       <c r="E10" t="n">
-        <v>3.24686919</v>
+        <v>3.19726144</v>
       </c>
       <c r="F10" t="n">
-        <v>0.00725225</v>
+        <v>0.00728126</v>
       </c>
       <c r="G10" t="n">
-        <v>0.0063133</v>
+        <v>0.00632601</v>
       </c>
       <c r="H10" t="n">
-        <v>0.04701933</v>
+        <v>0.04580960000000001</v>
       </c>
       <c r="I10" t="n">
-        <v>1.849084939940595</v>
+        <v>1.412053077576723</v>
       </c>
       <c r="J10" t="n">
-        <v>14.73880943304117</v>
+        <v>11.23250854654686</v>
       </c>
       <c r="K10" t="n">
-        <v>0.8159965815573966</v>
+        <v>0.662175724919601</v>
       </c>
       <c r="L10" t="n">
-        <v>0.0008214411744629697</v>
+        <v>0.0009135220495067073</v>
       </c>
       <c r="M10" t="n">
-        <v>0.001860064447740924</v>
+        <v>0.001703840324605493</v>
       </c>
       <c r="N10" t="n">
-        <v>0.02861437773330331</v>
+        <v>0.02170012876063707</v>
       </c>
       <c r="O10" t="n">
         <v>0.15</v>
@@ -941,40 +941,40 @@
         <v>1</v>
       </c>
       <c r="C11" t="n">
-        <v>13.327</v>
+        <v>12.66</v>
       </c>
       <c r="D11" t="n">
-        <v>82.93300000000001</v>
+        <v>80.422</v>
       </c>
       <c r="E11" t="n">
-        <v>2.1126916</v>
+        <v>2.16211396</v>
       </c>
       <c r="F11" t="n">
-        <v>0.004690980000000001</v>
+        <v>0.005118800000000001</v>
       </c>
       <c r="G11" t="n">
-        <v>0.007679880000000001</v>
+        <v>0.00795972</v>
       </c>
       <c r="H11" t="n">
-        <v>0.10770843</v>
+        <v>0.10568401</v>
       </c>
       <c r="I11" t="n">
-        <v>3.633631004143689</v>
+        <v>3.356138206877611</v>
       </c>
       <c r="J11" t="n">
-        <v>15.99544827022254</v>
+        <v>13.83876538667476</v>
       </c>
       <c r="K11" t="n">
-        <v>0.4027796196520463</v>
+        <v>0.3621626749625843</v>
       </c>
       <c r="L11" t="n">
-        <v>0.000741127323278065</v>
+        <v>0.0008798775736115477</v>
       </c>
       <c r="M11" t="n">
-        <v>0.001869444947039097</v>
+        <v>0.001979683931861364</v>
       </c>
       <c r="N11" t="n">
-        <v>0.05600667072591354</v>
+        <v>0.05539014756133772</v>
       </c>
       <c r="O11" t="n">
         <v>0.85</v>
@@ -988,40 +988,40 @@
         <v>1</v>
       </c>
       <c r="C12" t="n">
-        <v>5.6</v>
+        <v>5.608</v>
       </c>
       <c r="D12" t="n">
-        <v>55.818</v>
+        <v>55.843</v>
       </c>
       <c r="E12" t="n">
-        <v>3.224792820000001</v>
+        <v>3.180136210000001</v>
       </c>
       <c r="F12" t="n">
-        <v>0.00898761</v>
+        <v>0.00949055</v>
       </c>
       <c r="G12" t="n">
-        <v>0.005091549999999999</v>
+        <v>0.005367089999999999</v>
       </c>
       <c r="H12" t="n">
-        <v>0.03064861</v>
+        <v>0.03192714999999999</v>
       </c>
       <c r="I12" t="n">
-        <v>1.417041992323448</v>
+        <v>1.275916911073744</v>
       </c>
       <c r="J12" t="n">
-        <v>14.13374114092368</v>
+        <v>12.76625741273958</v>
       </c>
       <c r="K12" t="n">
-        <v>0.8269999832830698</v>
+        <v>0.7060770387562498</v>
       </c>
       <c r="L12" t="n">
-        <v>0.001463349233395391</v>
+        <v>0.001716747628488218</v>
       </c>
       <c r="M12" t="n">
-        <v>0.001717390324599224</v>
+        <v>0.001721453174772097</v>
       </c>
       <c r="N12" t="n">
-        <v>0.01804342584944124</v>
+        <v>0.01763455825424392</v>
       </c>
       <c r="O12" t="n">
         <v>0.15</v>
@@ -1035,40 +1035,40 @@
         <v>1</v>
       </c>
       <c r="C13" t="n">
-        <v>10.929</v>
+        <v>10.617</v>
       </c>
       <c r="D13" t="n">
-        <v>75.23699999999999</v>
+        <v>75.434</v>
       </c>
       <c r="E13" t="n">
-        <v>2.33108665</v>
+        <v>2.31641947</v>
       </c>
       <c r="F13" t="n">
-        <v>0.00538275</v>
+        <v>0.00557833</v>
       </c>
       <c r="G13" t="n">
-        <v>0.005766960000000001</v>
+        <v>0.00581731</v>
       </c>
       <c r="H13" t="n">
-        <v>0.06761159000000001</v>
+        <v>0.06624899999999999</v>
       </c>
       <c r="I13" t="n">
-        <v>3.428076823921936</v>
+        <v>3.315615222595092</v>
       </c>
       <c r="J13" t="n">
-        <v>14.84166790175909</v>
+        <v>14.03512125450395</v>
       </c>
       <c r="K13" t="n">
-        <v>0.4461306896167259</v>
+        <v>0.4230620195136572</v>
       </c>
       <c r="L13" t="n">
-        <v>0.0008616292372258745</v>
+        <v>0.0009005373276986239</v>
       </c>
       <c r="M13" t="n">
-        <v>0.001616815527773917</v>
+        <v>0.001655029542541971</v>
       </c>
       <c r="N13" t="n">
-        <v>0.04344393973930049</v>
+        <v>0.04440052480999975</v>
       </c>
       <c r="O13" t="n">
         <v>0.85</v>

</xml_diff>

<commit_message>
Addition of lambda parameter to proposed method (#16)
* added lambda param to new_cu

* 1000exp new_cu with lambda

* 100exp 30x30,50x50 new_cu with lambda+plots
</commit_message>
<xml_diff>
--- a/results/new_cu_diffgoal_path/15x15/new_cu_diffgoal_path_15x15_True_2_1000.xlsx
+++ b/results/new_cu_diffgoal_path/15x15/new_cu_diffgoal_path_15x15_True_2_1000.xlsx
@@ -518,40 +518,40 @@
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>54.069</v>
+        <v>54.114</v>
       </c>
       <c r="D2" t="n">
-        <v>54.069</v>
+        <v>54.114</v>
       </c>
       <c r="E2" t="n">
-        <v>3.17825061</v>
+        <v>3.16948242</v>
       </c>
       <c r="F2" t="n">
-        <v>0.00133787</v>
+        <v>0.00135841</v>
       </c>
       <c r="G2" t="n">
-        <v>0.07169933000000001</v>
+        <v>0.07295569</v>
       </c>
       <c r="H2" t="n">
-        <v>3.90818598</v>
+        <v>3.97650341</v>
       </c>
       <c r="I2" t="n">
-        <v>7.01023411751579</v>
+        <v>6.551482727285933</v>
       </c>
       <c r="J2" t="n">
-        <v>7.01023411751579</v>
+        <v>6.551482727285933</v>
       </c>
       <c r="K2" t="n">
-        <v>0.4138050426220387</v>
+        <v>0.3907925152580654</v>
       </c>
       <c r="L2" t="n">
-        <v>0.0001462147114412289</v>
+        <v>0.0001665157632159772</v>
       </c>
       <c r="M2" t="n">
-        <v>0.007553342586917089</v>
+        <v>0.008893789057972293</v>
       </c>
       <c r="N2" t="n">
-        <v>0.8345269440073902</v>
+        <v>0.8448462905931474</v>
       </c>
       <c r="O2" t="n">
         <v>0.15</v>
@@ -565,40 +565,40 @@
         <v>1</v>
       </c>
       <c r="C3" t="n">
-        <v>90.059</v>
+        <v>90.295</v>
       </c>
       <c r="D3" t="n">
-        <v>90.059</v>
+        <v>90.295</v>
       </c>
       <c r="E3" t="n">
-        <v>1.91107263</v>
+        <v>1.904231</v>
       </c>
       <c r="F3" t="n">
-        <v>0.0009027800000000001</v>
+        <v>0.000943</v>
       </c>
       <c r="G3" t="n">
-        <v>0.08052294</v>
+        <v>0.08433705000000001</v>
       </c>
       <c r="H3" t="n">
-        <v>7.314089279999999</v>
+        <v>7.67577954</v>
       </c>
       <c r="I3" t="n">
-        <v>12.08642215879458</v>
+        <v>11.89283037861107</v>
       </c>
       <c r="J3" t="n">
-        <v>12.08642215879458</v>
+        <v>11.89283037861107</v>
       </c>
       <c r="K3" t="n">
-        <v>0.2625993418524205</v>
+        <v>0.2527369708595069</v>
       </c>
       <c r="L3" t="n">
-        <v>0.0001330374780675377</v>
+        <v>0.0001822350394671936</v>
       </c>
       <c r="M3" t="n">
-        <v>0.01143470110434662</v>
+        <v>0.01559989991233196</v>
       </c>
       <c r="N3" t="n">
-        <v>1.735984363536182</v>
+        <v>2.005840126932154</v>
       </c>
       <c r="O3" t="n">
         <v>0.85</v>
@@ -612,40 +612,40 @@
         <v>1</v>
       </c>
       <c r="C4" t="n">
-        <v>27.046</v>
+        <v>27.812</v>
       </c>
       <c r="D4" t="n">
-        <v>54.078</v>
+        <v>55.605</v>
       </c>
       <c r="E4" t="n">
-        <v>3.25338949</v>
+        <v>3.104128</v>
       </c>
       <c r="F4" t="n">
-        <v>0.00252739</v>
+        <v>0.00264691</v>
       </c>
       <c r="G4" t="n">
-        <v>0.03362475000000001</v>
+        <v>0.0365285</v>
       </c>
       <c r="H4" t="n">
-        <v>0.93228702</v>
+        <v>1.03036605</v>
       </c>
       <c r="I4" t="n">
-        <v>5.543339481992115</v>
+        <v>4.142924066383527</v>
       </c>
       <c r="J4" t="n">
-        <v>11.08777952769872</v>
+        <v>8.279222217124053</v>
       </c>
       <c r="K4" t="n">
-        <v>0.6504573511170907</v>
+        <v>0.4427500415151439</v>
       </c>
       <c r="L4" t="n">
-        <v>0.0003879244427375946</v>
+        <v>0.0005123196495580892</v>
       </c>
       <c r="M4" t="n">
-        <v>0.005954293253245564</v>
+        <v>0.007658787474240003</v>
       </c>
       <c r="N4" t="n">
-        <v>0.341152542880503</v>
+        <v>0.3245784489303126</v>
       </c>
       <c r="O4" t="n">
         <v>0.15</v>
@@ -659,40 +659,40 @@
         <v>1</v>
       </c>
       <c r="C5" t="n">
-        <v>48.528</v>
+        <v>46.208</v>
       </c>
       <c r="D5" t="n">
-        <v>94.90900000000001</v>
+        <v>90.684</v>
       </c>
       <c r="E5" t="n">
-        <v>1.83129985</v>
+        <v>1.91382706</v>
       </c>
       <c r="F5" t="n">
-        <v>0.00154295</v>
+        <v>0.00166198</v>
       </c>
       <c r="G5" t="n">
-        <v>0.03694269</v>
+        <v>0.03787804</v>
       </c>
       <c r="H5" t="n">
-        <v>1.82836536</v>
+        <v>1.78094815</v>
       </c>
       <c r="I5" t="n">
-        <v>8.870394574081802</v>
+        <v>8.199632306998282</v>
       </c>
       <c r="J5" t="n">
-        <v>16.14848266842716</v>
+        <v>15.03117028311768</v>
       </c>
       <c r="K5" t="n">
-        <v>0.3064602012516939</v>
+        <v>0.3118262287250341</v>
       </c>
       <c r="L5" t="n">
-        <v>0.0001991221914984544</v>
+        <v>0.0002498441548279681</v>
       </c>
       <c r="M5" t="n">
-        <v>0.005546277946782235</v>
+        <v>0.006012809795764376</v>
       </c>
       <c r="N5" t="n">
-        <v>0.5994602327416799</v>
+        <v>0.5670590400082981</v>
       </c>
       <c r="O5" t="n">
         <v>0.85</v>
@@ -706,40 +706,40 @@
         <v>1</v>
       </c>
       <c r="C6" t="n">
-        <v>14.412</v>
+        <v>13.787</v>
       </c>
       <c r="D6" t="n">
-        <v>57.596</v>
+        <v>55.081</v>
       </c>
       <c r="E6" t="n">
-        <v>3.12679938</v>
+        <v>3.21703234</v>
       </c>
       <c r="F6" t="n">
-        <v>0.00429857</v>
+        <v>0.00435844</v>
       </c>
       <c r="G6" t="n">
-        <v>0.01526991</v>
+        <v>0.01488329</v>
       </c>
       <c r="H6" t="n">
-        <v>0.23138585</v>
+        <v>0.21439266</v>
       </c>
       <c r="I6" t="n">
-        <v>3.686983841821096</v>
+        <v>3.259794051356198</v>
       </c>
       <c r="J6" t="n">
-        <v>14.72894177209367</v>
+        <v>13.04640362887979</v>
       </c>
       <c r="K6" t="n">
-        <v>0.7895720725144161</v>
+        <v>0.656420880163054</v>
       </c>
       <c r="L6" t="n">
-        <v>0.0005525712534054681</v>
+        <v>0.0006457398441681808</v>
       </c>
       <c r="M6" t="n">
-        <v>0.003552977165510445</v>
+        <v>0.003572530258563019</v>
       </c>
       <c r="N6" t="n">
-        <v>0.1130356410103296</v>
+        <v>0.1058296747381356</v>
       </c>
       <c r="O6" t="n">
         <v>0.15</v>
@@ -753,40 +753,40 @@
         <v>1</v>
       </c>
       <c r="C7" t="n">
-        <v>25.316</v>
+        <v>24.351</v>
       </c>
       <c r="D7" t="n">
-        <v>93.711</v>
+        <v>90.449</v>
       </c>
       <c r="E7" t="n">
-        <v>1.85902356</v>
+        <v>1.92385209</v>
       </c>
       <c r="F7" t="n">
-        <v>0.00289656</v>
+        <v>0.00313757</v>
       </c>
       <c r="G7" t="n">
-        <v>0.01808876</v>
+        <v>0.01886938</v>
       </c>
       <c r="H7" t="n">
-        <v>0.47248698</v>
+        <v>0.4741455</v>
       </c>
       <c r="I7" t="n">
-        <v>5.427116877090229</v>
+        <v>5.201043150162268</v>
       </c>
       <c r="J7" t="n">
-        <v>16.34682530945069</v>
+        <v>15.66961824474151</v>
       </c>
       <c r="K7" t="n">
-        <v>0.3285856557732036</v>
+        <v>0.3288887290705498</v>
       </c>
       <c r="L7" t="n">
-        <v>0.0004357433173769148</v>
+        <v>0.000655178642931952</v>
       </c>
       <c r="M7" t="n">
-        <v>0.003690057640171463</v>
+        <v>0.004816035507926994</v>
       </c>
       <c r="N7" t="n">
-        <v>0.1946734041119848</v>
+        <v>0.2096587577418312</v>
       </c>
       <c r="O7" t="n">
         <v>0.85</v>
@@ -800,40 +800,40 @@
         <v>1</v>
       </c>
       <c r="C8" t="n">
-        <v>9.064</v>
+        <v>9.026</v>
       </c>
       <c r="D8" t="n">
-        <v>54.302</v>
+        <v>54.047</v>
       </c>
       <c r="E8" t="n">
-        <v>3.30350598</v>
+        <v>3.2465932</v>
       </c>
       <c r="F8" t="n">
-        <v>0.006348029999999999</v>
+        <v>0.00649477</v>
       </c>
       <c r="G8" t="n">
-        <v>0.00951017</v>
+        <v>0.00973795</v>
       </c>
       <c r="H8" t="n">
-        <v>0.09107359</v>
+        <v>0.09139376</v>
       </c>
       <c r="I8" t="n">
-        <v>2.335671072595488</v>
+        <v>1.854929854405488</v>
       </c>
       <c r="J8" t="n">
-        <v>14.01039211039745</v>
+        <v>11.1118073805868</v>
       </c>
       <c r="K8" t="n">
-        <v>0.7884226132480729</v>
+        <v>0.6145973977206909</v>
       </c>
       <c r="L8" t="n">
-        <v>0.001053982304309611</v>
+        <v>0.00153800201472472</v>
       </c>
       <c r="M8" t="n">
-        <v>0.002621400849453115</v>
+        <v>0.002884756439843269</v>
       </c>
       <c r="N8" t="n">
-        <v>0.04945781042690956</v>
+        <v>0.04736172435623935</v>
       </c>
       <c r="O8" t="n">
         <v>0.15</v>
@@ -847,40 +847,40 @@
         <v>1</v>
       </c>
       <c r="C9" t="n">
-        <v>17.186</v>
+        <v>16.821</v>
       </c>
       <c r="D9" t="n">
-        <v>87.908</v>
+        <v>86.29600000000001</v>
       </c>
       <c r="E9" t="n">
-        <v>1.98769757</v>
+        <v>2.01509231</v>
       </c>
       <c r="F9" t="n">
-        <v>0.00395629</v>
+        <v>0.004107620000000001</v>
       </c>
       <c r="G9" t="n">
-        <v>0.01114935</v>
+        <v>0.01131171</v>
       </c>
       <c r="H9" t="n">
-        <v>0.19931739</v>
+        <v>0.19793911</v>
       </c>
       <c r="I9" t="n">
-        <v>4.144705367403404</v>
+        <v>4.211020267309538</v>
       </c>
       <c r="J9" t="n">
-        <v>16.17173648873432</v>
+        <v>14.80106264615671</v>
       </c>
       <c r="K9" t="n">
-        <v>0.367135147468479</v>
+        <v>0.3395036868161016</v>
       </c>
       <c r="L9" t="n">
-        <v>0.0005622669116887282</v>
+        <v>0.000663986455896213</v>
       </c>
       <c r="M9" t="n">
-        <v>0.002346620613948025</v>
+        <v>0.00246834225531821</v>
       </c>
       <c r="N9" t="n">
-        <v>0.08966289475018573</v>
+        <v>0.09679939926366127</v>
       </c>
       <c r="O9" t="n">
         <v>0.85</v>
@@ -894,40 +894,40 @@
         <v>1</v>
       </c>
       <c r="C10" t="n">
-        <v>6.952</v>
+        <v>6.91</v>
       </c>
       <c r="D10" t="n">
-        <v>55.473</v>
+        <v>55.089</v>
       </c>
       <c r="E10" t="n">
-        <v>3.24686919</v>
+        <v>3.19726144</v>
       </c>
       <c r="F10" t="n">
-        <v>0.00725225</v>
+        <v>0.00728126</v>
       </c>
       <c r="G10" t="n">
-        <v>0.0063133</v>
+        <v>0.00632601</v>
       </c>
       <c r="H10" t="n">
-        <v>0.04701933</v>
+        <v>0.04580960000000001</v>
       </c>
       <c r="I10" t="n">
-        <v>1.849084939940595</v>
+        <v>1.412053077576723</v>
       </c>
       <c r="J10" t="n">
-        <v>14.73880943304117</v>
+        <v>11.23250854654686</v>
       </c>
       <c r="K10" t="n">
-        <v>0.8159965815573966</v>
+        <v>0.662175724919601</v>
       </c>
       <c r="L10" t="n">
-        <v>0.0008214411744629697</v>
+        <v>0.0009135220495067073</v>
       </c>
       <c r="M10" t="n">
-        <v>0.001860064447740924</v>
+        <v>0.001703840324605493</v>
       </c>
       <c r="N10" t="n">
-        <v>0.02861437773330331</v>
+        <v>0.02170012876063707</v>
       </c>
       <c r="O10" t="n">
         <v>0.15</v>
@@ -941,40 +941,40 @@
         <v>1</v>
       </c>
       <c r="C11" t="n">
-        <v>13.327</v>
+        <v>12.66</v>
       </c>
       <c r="D11" t="n">
-        <v>82.93300000000001</v>
+        <v>80.422</v>
       </c>
       <c r="E11" t="n">
-        <v>2.1126916</v>
+        <v>2.16211396</v>
       </c>
       <c r="F11" t="n">
-        <v>0.004690980000000001</v>
+        <v>0.005118800000000001</v>
       </c>
       <c r="G11" t="n">
-        <v>0.007679880000000001</v>
+        <v>0.00795972</v>
       </c>
       <c r="H11" t="n">
-        <v>0.10770843</v>
+        <v>0.10568401</v>
       </c>
       <c r="I11" t="n">
-        <v>3.633631004143689</v>
+        <v>3.356138206877611</v>
       </c>
       <c r="J11" t="n">
-        <v>15.99544827022254</v>
+        <v>13.83876538667476</v>
       </c>
       <c r="K11" t="n">
-        <v>0.4027796196520463</v>
+        <v>0.3621626749625843</v>
       </c>
       <c r="L11" t="n">
-        <v>0.000741127323278065</v>
+        <v>0.0008798775736115477</v>
       </c>
       <c r="M11" t="n">
-        <v>0.001869444947039097</v>
+        <v>0.001979683931861364</v>
       </c>
       <c r="N11" t="n">
-        <v>0.05600667072591354</v>
+        <v>0.05539014756133772</v>
       </c>
       <c r="O11" t="n">
         <v>0.85</v>
@@ -988,40 +988,40 @@
         <v>1</v>
       </c>
       <c r="C12" t="n">
-        <v>5.6</v>
+        <v>5.608</v>
       </c>
       <c r="D12" t="n">
-        <v>55.818</v>
+        <v>55.843</v>
       </c>
       <c r="E12" t="n">
-        <v>3.224792820000001</v>
+        <v>3.180136210000001</v>
       </c>
       <c r="F12" t="n">
-        <v>0.00898761</v>
+        <v>0.00949055</v>
       </c>
       <c r="G12" t="n">
-        <v>0.005091549999999999</v>
+        <v>0.005367089999999999</v>
       </c>
       <c r="H12" t="n">
-        <v>0.03064861</v>
+        <v>0.03192714999999999</v>
       </c>
       <c r="I12" t="n">
-        <v>1.417041992323448</v>
+        <v>1.275916911073744</v>
       </c>
       <c r="J12" t="n">
-        <v>14.13374114092368</v>
+        <v>12.76625741273958</v>
       </c>
       <c r="K12" t="n">
-        <v>0.8269999832830698</v>
+        <v>0.7060770387562498</v>
       </c>
       <c r="L12" t="n">
-        <v>0.001463349233395391</v>
+        <v>0.001716747628488218</v>
       </c>
       <c r="M12" t="n">
-        <v>0.001717390324599224</v>
+        <v>0.001721453174772097</v>
       </c>
       <c r="N12" t="n">
-        <v>0.01804342584944124</v>
+        <v>0.01763455825424392</v>
       </c>
       <c r="O12" t="n">
         <v>0.15</v>
@@ -1035,40 +1035,40 @@
         <v>1</v>
       </c>
       <c r="C13" t="n">
-        <v>10.929</v>
+        <v>10.617</v>
       </c>
       <c r="D13" t="n">
-        <v>75.23699999999999</v>
+        <v>75.434</v>
       </c>
       <c r="E13" t="n">
-        <v>2.33108665</v>
+        <v>2.31641947</v>
       </c>
       <c r="F13" t="n">
-        <v>0.00538275</v>
+        <v>0.00557833</v>
       </c>
       <c r="G13" t="n">
-        <v>0.005766960000000001</v>
+        <v>0.00581731</v>
       </c>
       <c r="H13" t="n">
-        <v>0.06761159000000001</v>
+        <v>0.06624899999999999</v>
       </c>
       <c r="I13" t="n">
-        <v>3.428076823921936</v>
+        <v>3.315615222595092</v>
       </c>
       <c r="J13" t="n">
-        <v>14.84166790175909</v>
+        <v>14.03512125450395</v>
       </c>
       <c r="K13" t="n">
-        <v>0.4461306896167259</v>
+        <v>0.4230620195136572</v>
       </c>
       <c r="L13" t="n">
-        <v>0.0008616292372258745</v>
+        <v>0.0009005373276986239</v>
       </c>
       <c r="M13" t="n">
-        <v>0.001616815527773917</v>
+        <v>0.001655029542541971</v>
       </c>
       <c r="N13" t="n">
-        <v>0.04344393973930049</v>
+        <v>0.04440052480999975</v>
       </c>
       <c r="O13" t="n">
         <v>0.85</v>

</xml_diff>